<commit_message>
Faster and more robust optimization 1/4/2018
</commit_message>
<xml_diff>
--- a/Studies/mass models conductance radiator area.xlsx
+++ b/Studies/mass models conductance radiator area.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>optimal table 10</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>mass</t>
+  </si>
+  <si>
+    <t>a_rad</t>
   </si>
 </sst>
 </file>
@@ -1748,6 +1751,833 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13151137357830273"/>
+                  <c:y val="4.5778288130650338E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$66:$B$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>84.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$66:$C$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A25-4A69-BDA9-CA48B52EDC26}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="511112712"/>
+        <c:axId val="511115336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="511112712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Panel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Area [m^2]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511115336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="511115336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>mass [kg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511112712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13438582677165353"/>
+                  <c:y val="8.3333333333333329E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$39:$U$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>574.21379999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$V$39:$V$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A55-4B83-9738-D9666B91C58D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="448617048"/>
+        <c:axId val="448618032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="448617048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>UA [W/K]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="448618032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="448618032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>mass [kg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="448617048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1828,6 +2658,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2345,6 +3255,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2986,6 +4928,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>425823</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>96370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>172570</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3252,10 +5254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N69" sqref="N69"/>
+    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3562,13 +5564,13 @@
         <v>1318.5</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>12</v>
       </c>
@@ -3576,7 +5578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>123</v>
       </c>
@@ -3590,7 +5592,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>260</v>
       </c>
@@ -3604,8 +5606,14 @@
         <f>P38*3.5136+58.244</f>
         <v>641.50160000000005</v>
       </c>
+      <c r="U38" t="s">
+        <v>9</v>
+      </c>
+      <c r="V38" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>410</v>
       </c>
@@ -3618,6 +5626,45 @@
       <c r="Q39">
         <f>P39*3.5136+58.244</f>
         <v>1899.3703999999998</v>
+      </c>
+      <c r="U39">
+        <v>574.21379999999999</v>
+      </c>
+      <c r="V39">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <f>(84.8+83.9)/2</f>
+        <v>84.35</v>
+      </c>
+      <c r="C66">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>